<commit_message>
calculadora de imposto de renda
</commit_message>
<xml_diff>
--- a/Dados/excel/relatorio_irpf.xlsx
+++ b/Dados/excel/relatorio_irpf.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,197 +436,61 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Rendimento Mensal (R$)</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>Rendimento Anual (R$)</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Dependentes</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Gastos com Saúde (R$)</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Gastos com Educação (R$)</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>INSS (R$)</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>IR Devido (R$)</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Rendimento Mensal (R$)</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>42000</v>
+        <v>10000</v>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>120000</v>
       </c>
       <c r="C2" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>500</v>
+        <v>5000</v>
       </c>
       <c r="E2" t="n">
-        <v>4000</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>1317.74</v>
-      </c>
-      <c r="G2" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>12000</v>
-      </c>
-      <c r="B3" t="n">
-        <v>5</v>
-      </c>
-      <c r="C3" t="n">
-        <v>1500</v>
-      </c>
-      <c r="D3" t="n">
-        <v>500</v>
-      </c>
-      <c r="E3" t="n">
-        <v>1350</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" t="n">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>12000</v>
-      </c>
-      <c r="B4" t="n">
-        <v>5</v>
-      </c>
-      <c r="C4" t="n">
-        <v>1500</v>
-      </c>
-      <c r="D4" t="n">
-        <v>500</v>
-      </c>
-      <c r="E4" t="n">
-        <v>2000</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" t="n">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>12000</v>
-      </c>
-      <c r="B5" t="n">
-        <v>5</v>
-      </c>
-      <c r="C5" t="n">
-        <v>3000</v>
-      </c>
-      <c r="D5" t="n">
-        <v>500</v>
-      </c>
-      <c r="E5" t="n">
-        <v>2000</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" t="n">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>12000</v>
-      </c>
-      <c r="B6" t="n">
-        <v>1</v>
-      </c>
-      <c r="C6" t="n">
-        <v>3000</v>
-      </c>
-      <c r="D6" t="n">
-        <v>500</v>
-      </c>
-      <c r="E6" t="n">
-        <v>2000</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" t="n">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>12000</v>
-      </c>
-      <c r="B7" t="n">
-        <v>5</v>
-      </c>
-      <c r="C7" t="n">
-        <v>500</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" t="n">
-        <v>2000</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0</v>
-      </c>
-      <c r="G7" t="n">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>12000</v>
-      </c>
-      <c r="B8" t="n">
-        <v>5</v>
-      </c>
-      <c r="C8" t="n">
-        <v>500</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0</v>
-      </c>
-      <c r="E8" t="n">
-        <v>1300</v>
-      </c>
-      <c r="F8" t="n">
-        <v>-0</v>
-      </c>
-      <c r="G8" t="n">
-        <v>1000</v>
+        <v>7000</v>
+      </c>
+      <c r="G2" t="n">
+        <v>20196</v>
       </c>
     </row>
   </sheetData>

</xml_diff>